<commit_message>
final check up rounds
</commit_message>
<xml_diff>
--- a/repswitch_V1L3.xlsx
+++ b/repswitch_V1L3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F92A83-9C3D-40EA-931C-F9B4CEC69682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E024B42-8697-4CAE-9C06-8F42DDA50949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10080" yWindow="600" windowWidth="12960" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="11" r:id="rId1"/>
@@ -1455,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C2ECCB-B040-46D7-A336-9E9BECBBD065}">
   <dimension ref="A1:Q409"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="A393" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>